<commit_message>
Updating Temporary entity spreadsheet.xlsx
</commit_message>
<xml_diff>
--- a/Temporary entity spreadsheet/Temporary entity spreadsheet.xlsx
+++ b/Temporary entity spreadsheet/Temporary entity spreadsheet.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -688,6 +688,54 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>GMHO:0000191</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>repeated measures study design</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>A study design in which measurements taken on the same study participants at two or more different times in different circumstances  are compared.</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>study design</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="inlineStr"/>
+      <c r="H5" s="2" t="inlineStr"/>
+      <c r="I5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="inlineStr"/>
+      <c r="K5" s="2" t="inlineStr"/>
+      <c r="L5" s="2" t="inlineStr"/>
+      <c r="M5" s="2" t="inlineStr"/>
+      <c r="N5" s="2" t="inlineStr"/>
+      <c r="O5" s="2" t="inlineStr"/>
+      <c r="P5" s="2" t="inlineStr"/>
+      <c r="Q5" s="2" t="inlineStr"/>
+      <c r="R5" s="2" t="inlineStr"/>
+      <c r="S5" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T5" s="2" t="inlineStr"/>
+      <c r="U5" s="2" t="inlineStr"/>
+      <c r="V5" s="2" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added external roots parent - temporarily
</commit_message>
<xml_diff>
--- a/Temporary entity spreadsheet/Temporary entity spreadsheet.xlsx
+++ b/Temporary entity spreadsheet/Temporary entity spreadsheet.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,22 +595,22 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000189</t>
+          <t>CHEBI:35470</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>health status attribute</t>
+          <t>central nervous system drug</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>A personal attribute that is the state of an individual's mental or physical condition.</t>
+          <t>A class of drugs producing both physiological and psychological effects through a variety of mechanisms involving the central nervous system.</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>personal attribute</t>
+          <t>function</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr"/>
@@ -636,29 +636,29 @@
       <c r="U3" s="2" t="inlineStr"/>
       <c r="V3" s="2" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>BG</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000190</t>
+          <t>CMO:0000000</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>person</t>
+          <t>clinical measurement</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>An extended organism that is a member of the species Homo sapiens.</t>
+          <t>A quantitative or qualitative value which is the result of an act of assessing a morphological or physiological state or property in a single individual or sample or a group of individuals or samples, based on direct observation or experimental manipulation.</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>extended organism</t>
+          <t>planned process</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr"/>
@@ -684,29 +684,29 @@
       <c r="U4" s="2" t="inlineStr"/>
       <c r="V4" s="2" t="inlineStr">
         <is>
-          <t>PS; BG</t>
+          <t>BG</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000191</t>
+          <t>GMHO:0000189</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>repeated measures study design</t>
+          <t>health status attribute</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>A study design in which measurements taken on the same study participants at two or more different times in different circumstances  are compared.</t>
+          <t>A personal attribute that is the state of an individual's mental or physical condition.</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>study design</t>
+          <t>personal attribute</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr"/>
@@ -732,6 +732,102 @@
       <c r="U5" s="2" t="inlineStr"/>
       <c r="V5" s="2" t="inlineStr">
         <is>
+          <t>PS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>GMHO:0000190</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>person</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>An extended organism that is a member of the species Homo sapiens.</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>extended organism</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="inlineStr"/>
+      <c r="H6" s="2" t="inlineStr"/>
+      <c r="I6" s="2" t="inlineStr"/>
+      <c r="J6" s="2" t="inlineStr"/>
+      <c r="K6" s="2" t="inlineStr"/>
+      <c r="L6" s="2" t="inlineStr"/>
+      <c r="M6" s="2" t="inlineStr"/>
+      <c r="N6" s="2" t="inlineStr"/>
+      <c r="O6" s="2" t="inlineStr"/>
+      <c r="P6" s="2" t="inlineStr"/>
+      <c r="Q6" s="2" t="inlineStr"/>
+      <c r="R6" s="2" t="inlineStr"/>
+      <c r="S6" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T6" s="2" t="inlineStr"/>
+      <c r="U6" s="2" t="inlineStr"/>
+      <c r="V6" s="2" t="inlineStr">
+        <is>
+          <t>PS; BG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>GMHO:0000191</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>repeated measures study design</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>A study design in which measurements taken on the same study participants at two or more different times in different circumstances  are compared.</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>study design</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr"/>
+      <c r="H7" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="inlineStr"/>
+      <c r="K7" s="2" t="inlineStr"/>
+      <c r="L7" s="2" t="inlineStr"/>
+      <c r="M7" s="2" t="inlineStr"/>
+      <c r="N7" s="2" t="inlineStr"/>
+      <c r="O7" s="2" t="inlineStr"/>
+      <c r="P7" s="2" t="inlineStr"/>
+      <c r="Q7" s="2" t="inlineStr"/>
+      <c r="R7" s="2" t="inlineStr"/>
+      <c r="S7" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T7" s="2" t="inlineStr"/>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="inlineStr">
+        <is>
           <t>BG</t>
         </is>
       </c>

</xml_diff>